<commit_message>
se agrego la clase 1 de aplicadas 2
</commit_message>
<xml_diff>
--- a/2015-2016/HORARIO LOAYZA.xlsx
+++ b/2015-2016/HORARIO LOAYZA.xlsx
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se realizo los avances
</commit_message>
<xml_diff>
--- a/2015-2016/HORARIO LOAYZA.xlsx
+++ b/2015-2016/HORARIO LOAYZA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>UNIVERSIDAD TÉCNICA DE MACHALA</t>
   </si>
@@ -155,9 +155,6 @@
     <t>11H30 12H30</t>
   </si>
   <si>
-    <t>C. CONTINUA ECONOMÍA</t>
-  </si>
-  <si>
     <t>12H30 13H30</t>
   </si>
   <si>
@@ -251,10 +248,10 @@
     <t>ABG. TERESA VIVANCO ALAÑA</t>
   </si>
   <si>
-    <t>          ECON. MARTHA AGUIRRE BENALCÁZAR, MBA.</t>
-  </si>
-  <si>
-    <t>SECRETARIA - ABOGADA </t>
+    <t>ECON. MARTHA AGUIRRE BENALCÁZAR, MBA.</t>
+  </si>
+  <si>
+    <t>SECRETARIA - ABOGADA</t>
   </si>
   <si>
     <t>SUBDECANA-UNIDAD ACADÉMICA DE CIENCIAS EMPRESARIALES</t>
@@ -462,7 +459,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -795,7 +792,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>43</v>
@@ -804,7 +801,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>38</v>
@@ -812,12 +809,12 @@
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>43</v>
@@ -826,7 +823,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -834,7 +831,7 @@
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -846,7 +843,7 @@
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -858,7 +855,7 @@
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -870,7 +867,7 @@
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -884,7 +881,7 @@
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -893,16 +890,16 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>40</v>
@@ -913,18 +910,18 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>40</v>
@@ -935,15 +932,15 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>35</v>
@@ -957,15 +954,15 @@
       <c r="F29" s="14"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="14"/>
@@ -973,7 +970,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,12 +982,12 @@
       <c r="F31" s="14"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1001,7 +998,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1010,10 +1007,10 @@
         <v>16</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -1027,10 +1024,10 @@
         <v>6</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -1044,16 +1041,16 @@
         <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1077,7 +1074,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1099,7 +1096,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1113,26 +1110,26 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F48" s="15"/>
     </row>

</xml_diff>